<commit_message>
inline list representation fixed
</commit_message>
<xml_diff>
--- a/project/excel/BICAN_schema.xlsx
+++ b/project/excel/BICAN_schema.xlsx
@@ -741,11 +741,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1042,11 +1037,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>